<commit_message>
no error but small results
</commit_message>
<xml_diff>
--- a/bbtnbc1.xlsx
+++ b/bbtnbc1.xlsx
@@ -11,10 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="37">
-  <si>
-    <t>Table 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
   <si>
     <t>ER</t>
   </si>
@@ -131,7 +128,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -141,6 +138,11 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="11"/>
@@ -165,7 +167,7 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,12 +183,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="12"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -220,8 +216,20 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="19"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="20"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -266,7 +274,9 @@
       <right style="thin">
         <color indexed="8"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
       <bottom style="thin">
         <color indexed="8"/>
       </bottom>
@@ -497,119 +507,173 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="8" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="10" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="7" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="8" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -633,12 +697,14 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffffff00"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ff92d050"/>
       <rgbColor rgb="ff00b0f0"/>
       <rgbColor rgb="ffe97132"/>
       <rgbColor rgb="ffa02b93"/>
       <rgbColor rgb="ffff0000"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -655,10 +721,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -835,11 +901,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -848,33 +917,33 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1113,12 +1182,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1399,7 +1468,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1667,11 +1736,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:X23"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
@@ -1683,984 +1750,979 @@
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
+      <c r="B1" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" t="s" s="4">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s" s="4">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s" s="5">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s" s="6">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s" s="7">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s" s="8">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s" s="9">
+        <v>19</v>
+      </c>
+      <c r="V1" t="s" s="10">
+        <v>20</v>
+      </c>
+      <c r="W1" s="11"/>
+      <c r="X1" s="12"/>
     </row>
     <row r="2" ht="22" customHeight="1">
-      <c r="A2" t="s" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s" s="3">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s" s="3">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s" s="3">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s" s="3">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s" s="3">
-        <v>7</v>
-      </c>
-      <c r="H2" t="s" s="3">
-        <v>8</v>
-      </c>
-      <c r="I2" t="s" s="3">
-        <v>9</v>
-      </c>
-      <c r="J2" t="s" s="3">
-        <v>10</v>
-      </c>
-      <c r="K2" t="s" s="3">
-        <v>11</v>
-      </c>
-      <c r="L2" s="4"/>
-      <c r="M2" t="s" s="5">
-        <v>12</v>
-      </c>
-      <c r="N2" t="s" s="5">
-        <v>13</v>
-      </c>
-      <c r="O2" t="s" s="5">
-        <v>14</v>
-      </c>
-      <c r="P2" t="s" s="6">
-        <v>15</v>
-      </c>
-      <c r="Q2" t="s" s="7">
-        <v>16</v>
-      </c>
-      <c r="R2" t="s" s="8">
-        <v>17</v>
-      </c>
-      <c r="S2" t="s" s="9">
-        <v>18</v>
-      </c>
-      <c r="T2" t="s" s="9">
-        <v>19</v>
-      </c>
-      <c r="U2" t="s" s="10">
-        <v>20</v>
-      </c>
-      <c r="V2" t="s" s="11">
+      <c r="A2" s="13">
+        <v>0.58894</v>
+      </c>
+      <c r="B2" s="14">
+        <v>0.54566</v>
+      </c>
+      <c r="C2" s="15">
+        <v>0.51245</v>
+      </c>
+      <c r="D2" s="16">
+        <v>1333.12456</v>
+      </c>
+      <c r="E2" s="16">
+        <v>45.1234</v>
+      </c>
+      <c r="F2" s="17">
+        <v>0.41235</v>
+      </c>
+      <c r="G2" s="18">
+        <v>12.3455</v>
+      </c>
+      <c r="H2" s="18">
+        <v>0.31113</v>
+      </c>
+      <c r="I2" s="18">
+        <v>988.1233999999999</v>
+      </c>
+      <c r="J2" s="18">
+        <v>4.2356</v>
+      </c>
+      <c r="K2" s="18">
+        <v>34.6342</v>
+      </c>
+      <c r="L2" t="s" s="19">
         <v>21</v>
       </c>
-      <c r="W2" s="12"/>
-      <c r="X2" s="13"/>
+      <c r="M2" s="20">
+        <v>20.1345</v>
+      </c>
+      <c r="N2" s="20">
+        <v>65.4892</v>
+      </c>
+      <c r="O2" s="20">
+        <v>405.134</v>
+      </c>
+      <c r="P2" s="20">
+        <v>140.6543</v>
+      </c>
+      <c r="Q2" s="20">
+        <v>52.54321</v>
+      </c>
+      <c r="R2" s="20">
+        <v>304.1245</v>
+      </c>
+      <c r="S2" s="20">
+        <v>70.124</v>
+      </c>
+      <c r="T2" s="20">
+        <v>85.11234</v>
+      </c>
+      <c r="U2" s="20">
+        <v>2.1451</v>
+      </c>
+      <c r="V2" s="20">
+        <v>15.123</v>
+      </c>
+      <c r="W2" t="s" s="21">
+        <v>22</v>
+      </c>
+      <c r="X2" t="s" s="22">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" ht="23" customHeight="1">
-      <c r="A3" s="14">
-        <v>0.58894</v>
-      </c>
-      <c r="B3" s="15">
-        <v>0.54566</v>
-      </c>
-      <c r="C3" s="16">
-        <v>0.51245</v>
-      </c>
-      <c r="D3" s="17">
-        <v>1333.12456</v>
-      </c>
-      <c r="E3" s="17">
-        <v>45.1234</v>
-      </c>
-      <c r="F3" s="18">
-        <v>0.41235</v>
-      </c>
-      <c r="G3" s="19">
-        <v>12.3455</v>
-      </c>
-      <c r="H3" s="19">
-        <v>0.31113</v>
-      </c>
-      <c r="I3" s="19">
-        <v>988.1233999999999</v>
-      </c>
-      <c r="J3" s="19">
-        <v>4.2356</v>
-      </c>
-      <c r="K3" s="19">
-        <v>34.6342</v>
-      </c>
-      <c r="L3" t="s" s="20">
-        <v>22</v>
-      </c>
-      <c r="M3" s="21">
-        <v>20.1345</v>
-      </c>
-      <c r="N3" s="21">
-        <v>65.4892</v>
-      </c>
-      <c r="O3" s="21">
-        <v>405.134</v>
-      </c>
-      <c r="P3" s="21">
-        <v>140.6543</v>
-      </c>
-      <c r="Q3" s="21">
-        <v>52.54321</v>
-      </c>
-      <c r="R3" s="21">
-        <v>304.1245</v>
-      </c>
-      <c r="S3" s="21">
-        <v>70.124</v>
-      </c>
-      <c r="T3" s="21">
-        <v>85.11234</v>
-      </c>
-      <c r="U3" s="21">
-        <v>2.1451</v>
-      </c>
-      <c r="V3" s="21">
-        <v>15.123</v>
-      </c>
-      <c r="W3" t="s" s="22">
+      <c r="A3" s="23">
+        <v>0.52134</v>
+      </c>
+      <c r="B3" s="24">
+        <v>0.53243</v>
+      </c>
+      <c r="C3" s="25">
+        <v>0.5124300000000001</v>
+      </c>
+      <c r="D3" s="26">
+        <v>1333.12355</v>
+      </c>
+      <c r="E3" s="26">
+        <v>30.1244</v>
+      </c>
+      <c r="F3" s="26">
+        <v>0.33245</v>
+      </c>
+      <c r="G3" s="26">
+        <v>0.51326</v>
+      </c>
+      <c r="H3" s="26">
+        <v>0.21354</v>
+      </c>
+      <c r="I3" s="26">
+        <v>1211.226</v>
+      </c>
+      <c r="J3" s="26">
+        <v>8.4245</v>
+      </c>
+      <c r="K3" s="26">
+        <v>21.3315</v>
+      </c>
+      <c r="L3" t="s" s="27">
+        <v>21</v>
+      </c>
+      <c r="M3" s="20">
+        <v>47.23852</v>
+      </c>
+      <c r="N3" s="20">
+        <v>50.6344</v>
+      </c>
+      <c r="O3" s="20">
+        <v>542.15432</v>
+      </c>
+      <c r="P3" s="20">
+        <v>124.1345</v>
+      </c>
+      <c r="Q3" s="20">
+        <v>70.14234999999999</v>
+      </c>
+      <c r="R3" s="20">
+        <v>280.1256</v>
+      </c>
+      <c r="S3" s="20">
+        <v>54.124356</v>
+      </c>
+      <c r="T3" s="20">
+        <v>98.14235600000001</v>
+      </c>
+      <c r="U3" s="20">
+        <v>1.243546</v>
+      </c>
+      <c r="V3" s="20">
+        <v>21.16543</v>
+      </c>
+      <c r="W3" t="s" s="28">
+        <v>24</v>
+      </c>
+      <c r="X3" t="s" s="29">
         <v>23</v>
-      </c>
-      <c r="X3" t="s" s="23">
-        <v>24</v>
       </c>
     </row>
     <row r="4" ht="23" customHeight="1">
-      <c r="A4" s="24">
-        <v>0.52134</v>
-      </c>
-      <c r="B4" s="25">
-        <v>0.53243</v>
-      </c>
-      <c r="C4" s="26">
-        <v>0.5124300000000001</v>
-      </c>
-      <c r="D4" s="27">
-        <v>1333.12355</v>
-      </c>
-      <c r="E4" s="27">
-        <v>30.1244</v>
-      </c>
-      <c r="F4" s="27">
-        <v>0.33245</v>
-      </c>
-      <c r="G4" s="27">
-        <v>0.51326</v>
-      </c>
-      <c r="H4" s="27">
-        <v>0.21354</v>
-      </c>
-      <c r="I4" s="27">
-        <v>1211.226</v>
-      </c>
-      <c r="J4" s="27">
-        <v>8.4245</v>
-      </c>
-      <c r="K4" s="27">
-        <v>21.3315</v>
-      </c>
-      <c r="L4" t="s" s="28">
-        <v>22</v>
-      </c>
-      <c r="M4" s="21">
-        <v>47.23852</v>
-      </c>
-      <c r="N4" s="21">
-        <v>50.6344</v>
-      </c>
-      <c r="O4" s="21">
-        <v>542.15432</v>
-      </c>
-      <c r="P4" s="21">
-        <v>124.1345</v>
-      </c>
-      <c r="Q4" s="21">
-        <v>70.14234999999999</v>
-      </c>
-      <c r="R4" s="21">
-        <v>280.1256</v>
-      </c>
-      <c r="S4" s="21">
-        <v>54.124356</v>
-      </c>
-      <c r="T4" s="21">
-        <v>98.14235600000001</v>
-      </c>
-      <c r="U4" s="21">
-        <v>1.243546</v>
-      </c>
-      <c r="V4" s="21">
-        <v>21.16543</v>
-      </c>
-      <c r="W4" t="s" s="29">
+      <c r="A4" s="23">
+        <v>0.51445</v>
+      </c>
+      <c r="B4" s="24">
+        <v>0.51245</v>
+      </c>
+      <c r="C4" s="25">
+        <v>0.52146</v>
+      </c>
+      <c r="D4" s="26">
+        <v>1333.124</v>
+      </c>
+      <c r="E4" s="26">
+        <v>40.1243</v>
+      </c>
+      <c r="F4" s="26">
+        <v>0.23254</v>
+      </c>
+      <c r="G4" s="26">
+        <v>0.41425</v>
+      </c>
+      <c r="H4" s="26">
+        <v>0.08774</v>
+      </c>
+      <c r="I4" s="26">
+        <v>1102.421</v>
+      </c>
+      <c r="J4" s="26">
+        <v>6.2453</v>
+      </c>
+      <c r="K4" s="26">
+        <v>11.2453</v>
+      </c>
+      <c r="L4" t="s" s="27">
         <v>25</v>
       </c>
-      <c r="X4" t="s" s="30">
-        <v>24</v>
+      <c r="M4" s="20">
+        <v>1.24564</v>
+      </c>
+      <c r="N4" s="20">
+        <v>1</v>
+      </c>
+      <c r="O4" s="20">
+        <v>123.1234</v>
+      </c>
+      <c r="P4" s="20">
+        <v>234.142354</v>
+      </c>
+      <c r="Q4" s="20">
+        <v>137.1243</v>
+      </c>
+      <c r="R4" s="20">
+        <v>503.132</v>
+      </c>
+      <c r="S4" s="20">
+        <v>50.142</v>
+      </c>
+      <c r="T4" s="20">
+        <v>80.1324</v>
+      </c>
+      <c r="U4" s="20">
+        <v>1.67654</v>
+      </c>
+      <c r="V4" s="20">
+        <v>16.145</v>
+      </c>
+      <c r="W4" t="s" s="28">
+        <v>26</v>
+      </c>
+      <c r="X4" t="s" s="29">
+        <v>27</v>
       </c>
     </row>
     <row r="5" ht="23" customHeight="1">
-      <c r="A5" s="24">
-        <v>0.51445</v>
-      </c>
-      <c r="B5" s="25">
-        <v>0.51245</v>
-      </c>
-      <c r="C5" s="26">
-        <v>0.52146</v>
-      </c>
-      <c r="D5" s="27">
-        <v>1333.124</v>
-      </c>
-      <c r="E5" s="27">
-        <v>40.1243</v>
-      </c>
-      <c r="F5" s="27">
-        <v>0.23254</v>
-      </c>
-      <c r="G5" s="27">
-        <v>0.41425</v>
-      </c>
-      <c r="H5" s="27">
-        <v>0.08774</v>
-      </c>
-      <c r="I5" s="27">
-        <v>1102.421</v>
-      </c>
-      <c r="J5" s="27">
-        <v>6.2453</v>
-      </c>
-      <c r="K5" s="27">
-        <v>11.2453</v>
-      </c>
-      <c r="L5" t="s" s="28">
-        <v>26</v>
-      </c>
-      <c r="M5" s="21">
-        <v>1.24564</v>
-      </c>
-      <c r="N5" s="21">
+      <c r="A5" s="23">
+        <v>0.51234</v>
+      </c>
+      <c r="B5" s="24">
+        <v>0.51425</v>
+      </c>
+      <c r="C5" s="25">
+        <v>0.53467</v>
+      </c>
+      <c r="D5" s="26">
+        <v>1333.1234</v>
+      </c>
+      <c r="E5" s="26">
+        <v>36.1245</v>
+      </c>
+      <c r="F5" s="26">
+        <v>0.92833</v>
+      </c>
+      <c r="G5" s="26">
+        <v>11.5323</v>
+      </c>
+      <c r="H5" s="26">
+        <v>0.31324</v>
+      </c>
+      <c r="I5" s="26">
+        <v>1200.123</v>
+      </c>
+      <c r="J5" s="26">
+        <v>8.353199999999999</v>
+      </c>
+      <c r="K5" s="26">
+        <v>17.3412</v>
+      </c>
+      <c r="L5" t="s" s="27">
+        <v>25</v>
+      </c>
+      <c r="M5" s="20">
+        <v>1.56987</v>
+      </c>
+      <c r="N5" s="20">
         <v>1</v>
       </c>
-      <c r="O5" s="21">
-        <v>123.1234</v>
-      </c>
-      <c r="P5" s="21">
-        <v>234.142354</v>
-      </c>
-      <c r="Q5" s="21">
-        <v>137.1243</v>
-      </c>
-      <c r="R5" s="21">
-        <v>503.132</v>
-      </c>
-      <c r="S5" s="21">
-        <v>50.142</v>
-      </c>
-      <c r="T5" s="21">
-        <v>80.1324</v>
-      </c>
-      <c r="U5" s="21">
-        <v>1.67654</v>
-      </c>
-      <c r="V5" s="21">
-        <v>16.145</v>
-      </c>
-      <c r="W5" t="s" s="29">
-        <v>27</v>
-      </c>
-      <c r="X5" t="s" s="30">
+      <c r="O5" s="20">
+        <v>217.14253467</v>
+      </c>
+      <c r="P5" s="20">
+        <v>142.3525</v>
+      </c>
+      <c r="Q5" s="20">
+        <v>46.2262</v>
+      </c>
+      <c r="R5" s="20">
+        <v>2356.215</v>
+      </c>
+      <c r="S5" s="20">
+        <v>63.2345</v>
+      </c>
+      <c r="T5" s="20">
+        <v>87.9876</v>
+      </c>
+      <c r="U5" s="20">
+        <v>1.23865</v>
+      </c>
+      <c r="V5" s="20">
+        <v>13.9873</v>
+      </c>
+      <c r="W5" t="s" s="28">
         <v>28</v>
+      </c>
+      <c r="X5" t="s" s="29">
+        <v>29</v>
       </c>
     </row>
     <row r="6" ht="23" customHeight="1">
-      <c r="A6" s="24">
+      <c r="A6" s="23">
         <v>0.51234</v>
       </c>
-      <c r="B6" s="25">
-        <v>0.51425</v>
-      </c>
-      <c r="C6" s="26">
-        <v>0.53467</v>
-      </c>
-      <c r="D6" s="27">
-        <v>1333.1234</v>
-      </c>
-      <c r="E6" s="27">
-        <v>36.1245</v>
-      </c>
-      <c r="F6" s="27">
-        <v>0.92833</v>
-      </c>
-      <c r="G6" s="27">
-        <v>11.5323</v>
-      </c>
-      <c r="H6" s="27">
-        <v>0.31324</v>
-      </c>
-      <c r="I6" s="27">
-        <v>1200.123</v>
-      </c>
-      <c r="J6" s="27">
-        <v>8.353199999999999</v>
-      </c>
-      <c r="K6" s="27">
-        <v>17.3412</v>
-      </c>
-      <c r="L6" t="s" s="28">
-        <v>26</v>
-      </c>
-      <c r="M6" s="21">
-        <v>1.56987</v>
-      </c>
-      <c r="N6" s="21">
-        <v>1</v>
-      </c>
-      <c r="O6" s="21">
-        <v>217.14253467</v>
-      </c>
-      <c r="P6" s="21">
-        <v>142.3525</v>
-      </c>
-      <c r="Q6" s="21">
-        <v>46.2262</v>
-      </c>
-      <c r="R6" s="21">
-        <v>2356.215</v>
-      </c>
-      <c r="S6" s="21">
-        <v>63.2345</v>
-      </c>
-      <c r="T6" s="21">
-        <v>87.9876</v>
-      </c>
-      <c r="U6" s="21">
-        <v>1.23865</v>
-      </c>
-      <c r="V6" s="21">
-        <v>13.9873</v>
-      </c>
-      <c r="W6" t="s" s="29">
-        <v>29</v>
-      </c>
-      <c r="X6" t="s" s="30">
+      <c r="B6" s="24">
+        <v>0.51256</v>
+      </c>
+      <c r="C6" s="25">
+        <v>0.56765</v>
+      </c>
+      <c r="D6" s="26">
+        <v>1333.5678</v>
+      </c>
+      <c r="E6" s="26">
+        <v>32.1232</v>
+      </c>
+      <c r="F6" s="26">
+        <v>0.56732</v>
+      </c>
+      <c r="G6" s="26">
+        <v>9.34122</v>
+      </c>
+      <c r="H6" s="26">
+        <v>0.77454</v>
+      </c>
+      <c r="I6" s="26">
+        <v>1001.452</v>
+      </c>
+      <c r="J6" s="26">
+        <v>5.3412</v>
+      </c>
+      <c r="K6" s="26">
+        <v>24.5224</v>
+      </c>
+      <c r="L6" t="s" s="27">
+        <v>21</v>
+      </c>
+      <c r="M6" s="20">
+        <v>2.23456</v>
+      </c>
+      <c r="N6" s="20">
+        <v>1.876</v>
+      </c>
+      <c r="O6" s="20">
+        <v>187.1276</v>
+      </c>
+      <c r="P6" s="20">
+        <v>111.123</v>
+      </c>
+      <c r="Q6" s="20">
+        <v>46.98765</v>
+      </c>
+      <c r="R6" s="20">
+        <v>432.092</v>
+      </c>
+      <c r="S6" s="20">
+        <v>190.123</v>
+      </c>
+      <c r="T6" s="20">
+        <v>200.132</v>
+      </c>
+      <c r="U6" s="20">
+        <v>1.092</v>
+      </c>
+      <c r="V6" s="20">
+        <v>15.6987</v>
+      </c>
+      <c r="W6" t="s" s="28">
         <v>30</v>
+      </c>
+      <c r="X6" t="s" s="29">
+        <v>31</v>
       </c>
     </row>
     <row r="7" ht="23" customHeight="1">
-      <c r="A7" s="24">
-        <v>0.51234</v>
-      </c>
-      <c r="B7" s="25">
-        <v>0.51256</v>
-      </c>
-      <c r="C7" s="26">
-        <v>0.56765</v>
-      </c>
-      <c r="D7" s="27">
-        <v>1333.5678</v>
-      </c>
-      <c r="E7" s="27">
-        <v>32.1232</v>
-      </c>
-      <c r="F7" s="27">
-        <v>0.56732</v>
-      </c>
-      <c r="G7" s="27">
-        <v>9.34122</v>
-      </c>
-      <c r="H7" s="27">
-        <v>0.77454</v>
-      </c>
-      <c r="I7" s="27">
-        <v>1001.452</v>
-      </c>
-      <c r="J7" s="27">
-        <v>5.3412</v>
-      </c>
-      <c r="K7" s="27">
-        <v>24.5224</v>
-      </c>
-      <c r="L7" t="s" s="28">
-        <v>22</v>
-      </c>
-      <c r="M7" s="21">
-        <v>2.23456</v>
-      </c>
-      <c r="N7" s="21">
-        <v>1.876</v>
-      </c>
-      <c r="O7" s="21">
-        <v>187.1276</v>
-      </c>
-      <c r="P7" s="21">
-        <v>111.123</v>
-      </c>
-      <c r="Q7" s="21">
-        <v>46.98765</v>
-      </c>
-      <c r="R7" s="21">
-        <v>432.092</v>
-      </c>
-      <c r="S7" s="21">
-        <v>190.123</v>
-      </c>
-      <c r="T7" s="21">
-        <v>200.132</v>
-      </c>
-      <c r="U7" s="21">
-        <v>1.092</v>
-      </c>
-      <c r="V7" s="21">
-        <v>15.6987</v>
-      </c>
-      <c r="W7" t="s" s="29">
-        <v>31</v>
-      </c>
-      <c r="X7" t="s" s="30">
+      <c r="A7" s="23">
+        <v>0.51242</v>
+      </c>
+      <c r="B7" s="24">
+        <v>0.56794</v>
+      </c>
+      <c r="C7" s="25">
+        <v>0.56587</v>
+      </c>
+      <c r="D7" s="26">
+        <v>1333.5654</v>
+      </c>
+      <c r="E7" s="26">
+        <v>31.1241</v>
+      </c>
+      <c r="F7" s="26">
+        <v>0.43223</v>
+      </c>
+      <c r="G7" s="26">
+        <v>0.21244</v>
+      </c>
+      <c r="H7" s="26">
+        <v>0.13123</v>
+      </c>
+      <c r="I7" s="26">
+        <v>1112.123</v>
+      </c>
+      <c r="J7" s="25">
+        <v>6.7214</v>
+      </c>
+      <c r="K7" s="25">
+        <v>45.7723</v>
+      </c>
+      <c r="L7" t="s" s="27">
+        <v>21</v>
+      </c>
+      <c r="M7" s="30">
+        <v>1.53256</v>
+      </c>
+      <c r="N7" s="30">
+        <v>1.6832</v>
+      </c>
+      <c r="O7" s="30">
+        <v>153.3462</v>
+      </c>
+      <c r="P7" s="30">
+        <v>134.252</v>
+      </c>
+      <c r="Q7" s="30">
+        <v>72.1362</v>
+      </c>
+      <c r="R7" s="30">
+        <v>1402.342</v>
+      </c>
+      <c r="S7" s="30">
+        <v>52.2451</v>
+      </c>
+      <c r="T7" s="30">
+        <v>92.12454</v>
+      </c>
+      <c r="U7" s="30">
+        <v>11.3521</v>
+      </c>
+      <c r="V7" s="30">
+        <v>21.532</v>
+      </c>
+      <c r="W7" t="s" s="28">
         <v>32</v>
+      </c>
+      <c r="X7" t="s" s="29">
+        <v>33</v>
       </c>
     </row>
     <row r="8" ht="22.65" customHeight="1">
-      <c r="A8" s="24">
-        <v>0.51242</v>
-      </c>
-      <c r="B8" s="25">
-        <v>0.56794</v>
-      </c>
-      <c r="C8" s="26">
-        <v>0.56587</v>
-      </c>
-      <c r="D8" s="27">
-        <v>1333.5654</v>
-      </c>
-      <c r="E8" s="27">
-        <v>31.1241</v>
-      </c>
-      <c r="F8" s="27">
-        <v>0.43223</v>
-      </c>
-      <c r="G8" s="27">
-        <v>0.21244</v>
-      </c>
-      <c r="H8" s="27">
-        <v>0.13123</v>
-      </c>
-      <c r="I8" s="27">
-        <v>1112.123</v>
-      </c>
-      <c r="J8" s="26">
-        <v>6.7214</v>
-      </c>
-      <c r="K8" s="26">
-        <v>45.7723</v>
-      </c>
-      <c r="L8" t="s" s="28">
-        <v>22</v>
+      <c r="A8" s="23">
+        <v>0.51256</v>
+      </c>
+      <c r="B8" s="24">
+        <v>0.54572</v>
+      </c>
+      <c r="C8" s="25">
+        <v>0.54673</v>
+      </c>
+      <c r="D8" s="26">
+        <v>1333.34568</v>
+      </c>
+      <c r="E8" s="26">
+        <v>14.6788</v>
+      </c>
+      <c r="F8" s="26">
+        <v>0.5642200000000001</v>
+      </c>
+      <c r="G8" s="26">
+        <v>0.64456</v>
+      </c>
+      <c r="H8" s="26">
+        <v>0.24242</v>
+      </c>
+      <c r="I8" s="26">
+        <v>1034.423</v>
+      </c>
+      <c r="J8" s="25">
+        <v>9.8124</v>
+      </c>
+      <c r="K8" s="25">
+        <v>13.1235</v>
+      </c>
+      <c r="L8" t="s" s="27">
+        <v>25</v>
       </c>
       <c r="M8" s="31">
-        <v>1.53256</v>
+        <v>1.75352</v>
       </c>
       <c r="N8" s="31">
-        <v>1.6832</v>
+        <v>1.0902</v>
       </c>
       <c r="O8" s="31">
-        <v>153.3462</v>
+        <v>180.2124</v>
       </c>
       <c r="P8" s="31">
-        <v>134.252</v>
-      </c>
-      <c r="Q8" s="31">
-        <v>72.1362</v>
-      </c>
-      <c r="R8" s="31">
-        <v>1402.342</v>
-      </c>
-      <c r="S8" s="31">
-        <v>52.2451</v>
-      </c>
-      <c r="T8" s="31">
-        <v>92.12454</v>
-      </c>
-      <c r="U8" s="31">
-        <v>11.3521</v>
-      </c>
-      <c r="V8" s="31">
-        <v>21.532</v>
-      </c>
-      <c r="W8" t="s" s="29">
-        <v>33</v>
-      </c>
-      <c r="X8" t="s" s="30">
+        <v>123.147</v>
+      </c>
+      <c r="Q8" s="32">
+        <v>67.315</v>
+      </c>
+      <c r="R8" s="32">
+        <v>403.2135</v>
+      </c>
+      <c r="S8" s="32">
+        <v>80.12520000000001</v>
+      </c>
+      <c r="T8" s="32">
+        <v>110.452</v>
+      </c>
+      <c r="U8" s="32">
+        <v>2.1562</v>
+      </c>
+      <c r="V8" s="32">
+        <v>50.1562</v>
+      </c>
+      <c r="W8" t="s" s="28">
         <v>34</v>
+      </c>
+      <c r="X8" t="s" s="29">
+        <v>35</v>
       </c>
     </row>
     <row r="9" ht="22.35" customHeight="1">
-      <c r="A9" s="24">
-        <v>0.51256</v>
-      </c>
-      <c r="B9" s="25">
-        <v>0.54572</v>
-      </c>
-      <c r="C9" s="26">
-        <v>0.54673</v>
-      </c>
-      <c r="D9" s="27">
-        <v>1333.34568</v>
-      </c>
-      <c r="E9" s="27">
-        <v>14.6788</v>
-      </c>
-      <c r="F9" s="27">
-        <v>0.5642200000000001</v>
-      </c>
-      <c r="G9" s="27">
-        <v>0.64456</v>
-      </c>
-      <c r="H9" s="27">
-        <v>0.24242</v>
-      </c>
-      <c r="I9" s="27">
-        <v>1034.423</v>
-      </c>
-      <c r="J9" s="26">
-        <v>9.8124</v>
-      </c>
-      <c r="K9" s="26">
-        <v>13.1235</v>
-      </c>
-      <c r="L9" t="s" s="28">
-        <v>26</v>
-      </c>
-      <c r="M9" s="32">
-        <v>1.75352</v>
-      </c>
-      <c r="N9" s="32">
-        <v>1.0902</v>
-      </c>
-      <c r="O9" s="32">
-        <v>180.2124</v>
-      </c>
-      <c r="P9" s="32">
-        <v>123.147</v>
-      </c>
-      <c r="Q9" s="32">
-        <v>67.315</v>
-      </c>
-      <c r="R9" s="32">
-        <v>403.2135</v>
-      </c>
-      <c r="S9" s="32">
-        <v>80.12520000000001</v>
-      </c>
-      <c r="T9" s="32">
-        <v>110.452</v>
-      </c>
-      <c r="U9" s="32">
-        <v>2.1562</v>
-      </c>
-      <c r="V9" s="32">
-        <v>50.1562</v>
-      </c>
-      <c r="W9" t="s" s="29">
-        <v>35</v>
-      </c>
-      <c r="X9" t="s" s="30">
-        <v>36</v>
-      </c>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="11"/>
+      <c r="X9" s="12"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="33"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="35"/>
-      <c r="P10" s="35"/>
-      <c r="Q10" s="35"/>
-      <c r="R10" s="35"/>
-      <c r="S10" s="35"/>
-      <c r="T10" s="35"/>
-      <c r="U10" s="35"/>
-      <c r="V10" s="35"/>
-      <c r="W10" s="35"/>
-      <c r="X10" s="35"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="41"/>
+      <c r="P10" s="41"/>
+      <c r="Q10" s="41"/>
+      <c r="R10" s="41"/>
+      <c r="S10" s="41"/>
+      <c r="T10" s="41"/>
+      <c r="U10" s="41"/>
+      <c r="V10" s="41"/>
+      <c r="W10" s="21"/>
+      <c r="X10" s="22"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="33"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="35"/>
-      <c r="Q11" s="35"/>
-      <c r="R11" s="35"/>
-      <c r="S11" s="35"/>
-      <c r="T11" s="35"/>
-      <c r="U11" s="35"/>
-      <c r="V11" s="35"/>
-      <c r="W11" s="35"/>
-      <c r="X11" s="35"/>
+      <c r="A11" s="42"/>
+      <c r="B11" s="43"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="45"/>
+      <c r="L11" s="27"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="41"/>
+      <c r="Q11" s="41"/>
+      <c r="R11" s="41"/>
+      <c r="S11" s="41"/>
+      <c r="T11" s="41"/>
+      <c r="U11" s="41"/>
+      <c r="V11" s="41"/>
+      <c r="W11" s="28"/>
+      <c r="X11" s="29"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="33"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
-      <c r="N12" s="35"/>
-      <c r="O12" s="35"/>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="35"/>
-      <c r="R12" s="35"/>
-      <c r="S12" s="35"/>
-      <c r="T12" s="35"/>
-      <c r="U12" s="35"/>
-      <c r="V12" s="35"/>
-      <c r="W12" s="35"/>
-      <c r="X12" s="35"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="45"/>
+      <c r="H12" s="45"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="41"/>
+      <c r="P12" s="41"/>
+      <c r="Q12" s="41"/>
+      <c r="R12" s="41"/>
+      <c r="S12" s="41"/>
+      <c r="T12" s="41"/>
+      <c r="U12" s="41"/>
+      <c r="V12" s="41"/>
+      <c r="W12" s="28"/>
+      <c r="X12" s="29"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="33"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="35"/>
-      <c r="M13" s="35"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="35"/>
-      <c r="Q13" s="35"/>
-      <c r="R13" s="35"/>
-      <c r="S13" s="35"/>
-      <c r="T13" s="35"/>
-      <c r="U13" s="35"/>
-      <c r="V13" s="35"/>
-      <c r="W13" s="35"/>
-      <c r="X13" s="35"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="44"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="45"/>
+      <c r="H13" s="45"/>
+      <c r="I13" s="45"/>
+      <c r="J13" s="45"/>
+      <c r="K13" s="45"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
+      <c r="P13" s="41"/>
+      <c r="Q13" s="41"/>
+      <c r="R13" s="41"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
+      <c r="U13" s="41"/>
+      <c r="V13" s="41"/>
+      <c r="W13" s="28"/>
+      <c r="X13" s="29"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="33"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="35"/>
-      <c r="I14" s="35"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="35"/>
-      <c r="O14" s="35"/>
-      <c r="P14" s="35"/>
-      <c r="Q14" s="35"/>
-      <c r="R14" s="35"/>
-      <c r="S14" s="35"/>
-      <c r="T14" s="35"/>
-      <c r="U14" s="35"/>
-      <c r="V14" s="35"/>
-      <c r="W14" s="35"/>
-      <c r="X14" s="35"/>
+      <c r="A14" s="42"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="45"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="45"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="27"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="41"/>
+      <c r="Q14" s="41"/>
+      <c r="R14" s="41"/>
+      <c r="S14" s="41"/>
+      <c r="T14" s="41"/>
+      <c r="U14" s="41"/>
+      <c r="V14" s="41"/>
+      <c r="W14" s="28"/>
+      <c r="X14" s="29"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="33"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-      <c r="O15" s="35"/>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="35"/>
-      <c r="S15" s="35"/>
-      <c r="T15" s="35"/>
-      <c r="U15" s="35"/>
-      <c r="V15" s="35"/>
-      <c r="W15" s="35"/>
-      <c r="X15" s="35"/>
+      <c r="A15" s="42"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="46"/>
+      <c r="N15" s="46"/>
+      <c r="O15" s="46"/>
+      <c r="P15" s="46"/>
+      <c r="Q15" s="46"/>
+      <c r="R15" s="46"/>
+      <c r="S15" s="46"/>
+      <c r="T15" s="46"/>
+      <c r="U15" s="46"/>
+      <c r="V15" s="46"/>
+      <c r="W15" s="28"/>
+      <c r="X15" s="29"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="33"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="35"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="35"/>
-      <c r="S16" s="35"/>
-      <c r="T16" s="35"/>
-      <c r="U16" s="35"/>
-      <c r="V16" s="35"/>
-      <c r="W16" s="35"/>
-      <c r="X16" s="35"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="47"/>
+      <c r="O16" s="47"/>
+      <c r="P16" s="47"/>
+      <c r="Q16" s="48"/>
+      <c r="R16" s="48"/>
+      <c r="S16" s="48"/>
+      <c r="T16" s="48"/>
+      <c r="U16" s="48"/>
+      <c r="V16" s="48"/>
+      <c r="W16" s="28"/>
+      <c r="X16" s="29"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="33"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35"/>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="35"/>
-      <c r="S17" s="35"/>
-      <c r="T17" s="35"/>
-      <c r="U17" s="35"/>
-      <c r="V17" s="35"/>
-      <c r="W17" s="35"/>
-      <c r="X17" s="35"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="33"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="11"/>
+      <c r="X17" s="12"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="33"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="35"/>
-      <c r="S18" s="35"/>
-      <c r="T18" s="35"/>
-      <c r="U18" s="35"/>
-      <c r="V18" s="35"/>
-      <c r="W18" s="35"/>
-      <c r="X18" s="35"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="41"/>
+      <c r="Q18" s="41"/>
+      <c r="R18" s="41"/>
+      <c r="S18" s="41"/>
+      <c r="T18" s="41"/>
+      <c r="U18" s="41"/>
+      <c r="V18" s="41"/>
+      <c r="W18" s="21"/>
+      <c r="X18" s="22"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="33"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="35"/>
-      <c r="L19" s="35"/>
-      <c r="M19" s="35"/>
-      <c r="N19" s="35"/>
-      <c r="O19" s="35"/>
-      <c r="P19" s="35"/>
-      <c r="Q19" s="35"/>
-      <c r="R19" s="35"/>
-      <c r="S19" s="35"/>
-      <c r="T19" s="35"/>
-      <c r="U19" s="35"/>
-      <c r="V19" s="35"/>
-      <c r="W19" s="35"/>
-      <c r="X19" s="35"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="45"/>
+      <c r="H19" s="45"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="45"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="41"/>
+      <c r="P19" s="41"/>
+      <c r="Q19" s="41"/>
+      <c r="R19" s="41"/>
+      <c r="S19" s="41"/>
+      <c r="T19" s="41"/>
+      <c r="U19" s="41"/>
+      <c r="V19" s="41"/>
+      <c r="W19" s="28"/>
+      <c r="X19" s="29"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="33"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="35"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="35"/>
-      <c r="N20" s="35"/>
-      <c r="O20" s="35"/>
-      <c r="P20" s="35"/>
-      <c r="Q20" s="35"/>
-      <c r="R20" s="35"/>
-      <c r="S20" s="35"/>
-      <c r="T20" s="35"/>
-      <c r="U20" s="35"/>
-      <c r="V20" s="35"/>
-      <c r="W20" s="35"/>
-      <c r="X20" s="35"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="45"/>
+      <c r="H20" s="45"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
+      <c r="K20" s="45"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="41"/>
+      <c r="P20" s="41"/>
+      <c r="Q20" s="41"/>
+      <c r="R20" s="41"/>
+      <c r="S20" s="41"/>
+      <c r="T20" s="41"/>
+      <c r="U20" s="41"/>
+      <c r="V20" s="41"/>
+      <c r="W20" s="28"/>
+      <c r="X20" s="29"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="33"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="35"/>
-      <c r="N21" s="35"/>
-      <c r="O21" s="35"/>
-      <c r="P21" s="35"/>
-      <c r="Q21" s="35"/>
-      <c r="R21" s="35"/>
-      <c r="S21" s="35"/>
-      <c r="T21" s="35"/>
-      <c r="U21" s="35"/>
-      <c r="V21" s="35"/>
-      <c r="W21" s="35"/>
-      <c r="X21" s="35"/>
+      <c r="A21" s="42"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
+      <c r="I21" s="45"/>
+      <c r="J21" s="45"/>
+      <c r="K21" s="45"/>
+      <c r="L21" s="27"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="41"/>
+      <c r="P21" s="41"/>
+      <c r="Q21" s="41"/>
+      <c r="R21" s="41"/>
+      <c r="S21" s="41"/>
+      <c r="T21" s="41"/>
+      <c r="U21" s="41"/>
+      <c r="V21" s="41"/>
+      <c r="W21" s="28"/>
+      <c r="X21" s="29"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="33"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="35"/>
-      <c r="N22" s="35"/>
-      <c r="O22" s="35"/>
-      <c r="P22" s="35"/>
-      <c r="Q22" s="35"/>
-      <c r="R22" s="35"/>
-      <c r="S22" s="35"/>
-      <c r="T22" s="35"/>
-      <c r="U22" s="35"/>
-      <c r="V22" s="35"/>
-      <c r="W22" s="35"/>
-      <c r="X22" s="35"/>
+      <c r="A22" s="42"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="45"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="45"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="45"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="41"/>
+      <c r="P22" s="41"/>
+      <c r="Q22" s="41"/>
+      <c r="R22" s="41"/>
+      <c r="S22" s="41"/>
+      <c r="T22" s="41"/>
+      <c r="U22" s="41"/>
+      <c r="V22" s="41"/>
+      <c r="W22" s="28"/>
+      <c r="X22" s="29"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="33"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="35"/>
-      <c r="L23" s="35"/>
-      <c r="M23" s="35"/>
-      <c r="N23" s="35"/>
-      <c r="O23" s="35"/>
-      <c r="P23" s="35"/>
-      <c r="Q23" s="35"/>
-      <c r="R23" s="35"/>
-      <c r="S23" s="35"/>
-      <c r="T23" s="35"/>
-      <c r="U23" s="35"/>
-      <c r="V23" s="35"/>
-      <c r="W23" s="35"/>
-      <c r="X23" s="35"/>
+      <c r="A23" s="42"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="44"/>
+      <c r="K23" s="44"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="46"/>
+      <c r="N23" s="46"/>
+      <c r="O23" s="46"/>
+      <c r="P23" s="46"/>
+      <c r="Q23" s="46"/>
+      <c r="R23" s="46"/>
+      <c r="S23" s="46"/>
+      <c r="T23" s="46"/>
+      <c r="U23" s="46"/>
+      <c r="V23" s="46"/>
+      <c r="W23" s="28"/>
+      <c r="X23" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:X1"/>
-  </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>